<commit_message>
more utility methods added
</commit_message>
<xml_diff>
--- a/DemoProject/src/test/java/com/demo/testdata/web/testdatatemp.xlsx
+++ b/DemoProject/src/test/java/com/demo/testdata/web/testdatatemp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" state="visible" r:id="rId2"/>
@@ -54,10 +54,10 @@
     <t xml:space="preserve">Patient_Gender</t>
   </si>
   <si>
-    <t xml:space="preserve">Pamella Halpert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9034500898</t>
+    <t xml:space="preserve">Jan Levinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9034500777</t>
   </si>
   <si>
     <t xml:space="preserve">Female</t>
@@ -275,7 +275,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -311,12 +311,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -374,7 +368,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -411,10 +405,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +428,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.88"/>
@@ -479,11 +469,11 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.5"/>
@@ -542,7 +532,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.24"/>
@@ -600,7 +590,7 @@
       <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
@@ -640,7 +630,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.63"/>
@@ -775,7 +765,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
@@ -843,17 +833,17 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.61"/>
@@ -875,10 +865,10 @@
       <c r="E1" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>69</v>
       </c>
     </row>
@@ -895,13 +885,13 @@
       <c r="D2" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -927,7 +917,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -961,7 +951,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>